<commit_message>
Finished creating packages and empty classes (except DaoDB classes). Index page is finished and other html pages have blank content. Web server runs fine.
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -5,16 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C6749-1A4B-45D9-B91E-CF87A05A59D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6632849C-2C5E-43C3-8A65-6D359DD6D60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Report 8-27" sheetId="1" r:id="rId1"/>
     <sheet name="Status Report 8-28" sheetId="3" r:id="rId2"/>
+    <sheet name="Next Steps" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="48">
   <si>
     <t>Project</t>
   </si>
@@ -220,6 +221,27 @@
   </si>
   <si>
     <t>Created test-data creation scripts</t>
+  </si>
+  <si>
+    <t>Create test cases</t>
+  </si>
+  <si>
+    <t>Set up environment</t>
+  </si>
+  <si>
+    <t>Document necessary 3rd party endpoints and format</t>
+  </si>
+  <si>
+    <t>Create interface methods</t>
+  </si>
+  <si>
+    <t>Create model class methods</t>
+  </si>
+  <si>
+    <t>Create service and controller method outlines</t>
+  </si>
+  <si>
+    <t>Create static html backbone</t>
   </si>
 </sst>
 </file>
@@ -327,7 +349,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +484,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -543,6 +571,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -946,15 +989,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1003,9 +1046,9 @@
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1015,9 +1058,9 @@
         <v>21</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1488,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11D01E5-4373-4DAD-AA18-4DB1BB006D5A}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1503,15 +1546,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1560,9 +1603,9 @@
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1572,9 +1615,9 @@
         <v>21</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1658,178 +1701,176 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="27">
-        <v>0</v>
-      </c>
-      <c r="E19" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="27">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24">
+        <v>44436</v>
+      </c>
       <c r="F20" s="24"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="27">
-        <v>0</v>
-      </c>
-      <c r="E21" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="24">
-        <v>44436</v>
+        <v>44440</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="24">
-        <v>44440</v>
+        <v>44436</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="27">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24">
+        <v>44440</v>
+      </c>
       <c r="F24" s="24"/>
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="27">
-        <v>0</v>
-      </c>
-      <c r="E25" s="24">
-        <v>44439</v>
-      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="24">
-        <v>44437</v>
+        <v>44439</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1844,22 +1885,22 @@
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="24">
-        <v>44438</v>
+        <v>44437</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1867,53 +1908,53 @@
         <v>0</v>
       </c>
       <c r="E29" s="24">
-        <v>44439</v>
+        <v>44438</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="27">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="28">
-        <v>0</v>
-      </c>
-      <c r="E30" s="25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="28">
+        <v>0</v>
+      </c>
+      <c r="E31" s="25">
         <v>44439</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="27">
-        <v>0</v>
-      </c>
-      <c r="E32" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D32" s="27"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -1921,14 +1962,14 @@
         <v>0</v>
       </c>
       <c r="E33" s="24">
-        <v>44438</v>
+        <v>44440</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -1936,38 +1977,38 @@
         <v>0</v>
       </c>
       <c r="E34" s="24">
-        <v>44440</v>
+        <v>44438</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="24"/>
+      <c r="D35" s="27">
+        <v>0</v>
+      </c>
+      <c r="E35" s="24">
+        <v>44440</v>
+      </c>
       <c r="F35" s="24"/>
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="28">
-        <v>0</v>
-      </c>
-      <c r="E36" s="25">
-        <v>44440</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1975,19 +2016,25 @@
         <v>0</v>
       </c>
       <c r="E37" s="25">
-        <v>44441</v>
+        <v>44440</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="A38" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="28">
+        <v>0</v>
+      </c>
+      <c r="E38" s="25">
+        <v>44441</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
@@ -2025,16 +2072,24 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
     </row>
-    <row r="43" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+    </row>
     <row r="45" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2043,6 +2098,7 @@
     <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
@@ -2057,4 +2113,670 @@
   </headerFooter>
   <legacyDrawingHF r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2755D9C-88E6-44E4-9B88-8D336F63A0A1}">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.375" style="2" customWidth="1"/>
+    <col min="4" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22">
+        <v>44436</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27">
+        <v>1</v>
+      </c>
+      <c r="E19" s="34">
+        <v>44436</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="30">
+        <v>0</v>
+      </c>
+      <c r="E20" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F20" s="32"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="30">
+        <v>0</v>
+      </c>
+      <c r="E21" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="30">
+        <v>0</v>
+      </c>
+      <c r="E22" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="30">
+        <v>0</v>
+      </c>
+      <c r="E23" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="30">
+        <v>0</v>
+      </c>
+      <c r="E24" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="30">
+        <v>0</v>
+      </c>
+      <c r="E25" s="32">
+        <v>44436</v>
+      </c>
+      <c r="F25" s="32"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <v>44436</v>
+      </c>
+      <c r="F26" s="24"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="27">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="30">
+        <v>0</v>
+      </c>
+      <c r="E29" s="32">
+        <v>44438</v>
+      </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="27">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="27">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="27">
+        <v>0</v>
+      </c>
+      <c r="E32" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="27">
+        <v>0</v>
+      </c>
+      <c r="E33" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="27">
+        <v>0</v>
+      </c>
+      <c r="E34" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F34" s="24"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="27">
+        <v>0</v>
+      </c>
+      <c r="E35" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F35" s="24"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="28">
+        <v>0</v>
+      </c>
+      <c r="E36" s="25">
+        <v>44440</v>
+      </c>
+      <c r="F36" s="25"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="27">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="27">
+        <v>0</v>
+      </c>
+      <c r="E38" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="27">
+        <v>0</v>
+      </c>
+      <c r="E39" s="24">
+        <v>44441</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+    </row>
+    <row r="49" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:G43">
+    <sortCondition ref="E19:E43"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E5:G6"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"&amp;10Status Report&amp;R&amp;"Arial,Regular"&amp;8v1.0</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;8&amp;G_x000D_Copyright 2018 GoLeanSixSigma.com. All Rights Reserved.</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added dependency necessary for parsing JSON objects and arrays when performing 3rd party API calls
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15187FAA-49AE-4E4B-92BF-69332D69ACE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25DDE95-98CF-4DEB-9DAB-6442CE41DE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -588,6 +588,9 @@
     <xf numFmtId="16" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,7 +600,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -997,15 +1006,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1054,9 +1063,9 @@
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1066,9 +1075,9 @@
         <v>21</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1542,7 +1551,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1554,15 +1563,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1611,9 +1620,9 @@
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1623,9 +1632,9 @@
         <v>21</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -2128,7 +2137,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2140,15 +2149,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -2197,9 +2206,9 @@
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -2209,9 +2218,9 @@
         <v>21</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -2372,11 +2381,11 @@
       <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="27">
         <v>1</v>
       </c>
@@ -2384,7 +2393,7 @@
         <v>44436</v>
       </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="38"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
@@ -2432,19 +2441,19 @@
       <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="30">
-        <v>0</v>
-      </c>
-      <c r="E24" s="32">
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40">
+        <v>0</v>
+      </c>
+      <c r="E24" s="41">
         <v>44436</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="31"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
@@ -2462,11 +2471,11 @@
       <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="27">
         <v>1</v>
       </c>
@@ -2474,14 +2483,14 @@
         <v>44436</v>
       </c>
       <c r="F26" s="34"/>
-      <c r="G26" s="38"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="27">
         <v>1</v>
       </c>
@@ -2489,14 +2498,14 @@
         <v>44437</v>
       </c>
       <c r="F27" s="34"/>
-      <c r="G27" s="38"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="27">
         <v>1</v>
       </c>
@@ -2504,18 +2513,18 @@
         <v>44437</v>
       </c>
       <c r="F28" s="34"/>
-      <c r="G28" s="38"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
-      <c r="D29" s="30">
-        <v>0</v>
-      </c>
-      <c r="E29" s="32">
+      <c r="D29" s="40">
+        <v>0</v>
+      </c>
+      <c r="E29" s="41">
         <v>44438</v>
       </c>
       <c r="F29" s="32"/>

</xml_diff>

<commit_message>
Created interfaces for worddao and wordvariantdao. Finished creating unit tests for wordvariantdaodb. Started for worddaodb.
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25DDE95-98CF-4DEB-9DAB-6442CE41DE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C5390E-D1DE-4BC7-B301-524387111FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13125" yWindow="4095" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Report 8-27" sheetId="1" r:id="rId1"/>
-    <sheet name="Status Report 8-28" sheetId="3" r:id="rId2"/>
-    <sheet name="Next Steps" sheetId="4" r:id="rId3"/>
+    <sheet name="Status Report 8-30" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>Project</t>
   </si>
@@ -142,9 +141,6 @@
     <t>Health</t>
   </si>
   <si>
-    <t>Due Date</t>
-  </si>
-  <si>
     <t>Comment/Status</t>
   </si>
   <si>
@@ -223,25 +219,19 @@
     <t>Created test-data creation scripts</t>
   </si>
   <si>
-    <t>Create test cases</t>
-  </si>
-  <si>
     <t>Set up environment</t>
   </si>
   <si>
-    <t>Document necessary 3rd party endpoints and format</t>
-  </si>
-  <si>
-    <t>Create interface methods</t>
-  </si>
-  <si>
-    <t>Create model class methods</t>
-  </si>
-  <si>
-    <t>Create service and controller method outlines</t>
-  </si>
-  <si>
-    <t>Create static html backbone</t>
+    <t>Documented necessary endpoints and JSON format for 3rd party API calls</t>
+  </si>
+  <si>
+    <t>Created backbone of HTML pages</t>
+  </si>
+  <si>
+    <t>Due Date (EOD)</t>
+  </si>
+  <si>
+    <t>Created model classes in Netbeans</t>
   </si>
 </sst>
 </file>
@@ -349,7 +339,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,12 +385,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +468,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -573,24 +557,6 @@
     <xf numFmtId="9" fontId="9" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,13 +566,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -655,6 +615,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFF2F2F2"/>
       <color rgb="FF92D050"/>
     </mruColors>
   </colors>
@@ -993,28 +954,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="37.375" style="2" customWidth="1"/>
-    <col min="4" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1"/>
+    <col min="6" max="7" width="15.625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1048,7 +1011,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1058,26 +1021,26 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1111,10 +1074,10 @@
     </row>
     <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -1124,10 +1087,10 @@
     </row>
     <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1155,7 +1118,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>10</v>
@@ -1198,16 +1161,16 @@
         <v>13</v>
       </c>
       <c r="E17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>15</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1230,8 +1193,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>31</v>
+      <c r="A20" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1246,7 +1209,7 @@
     </row>
     <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -1261,7 +1224,7 @@
     </row>
     <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1284,8 +1247,8 @@
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>32</v>
+      <c r="A24" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1300,7 +1263,7 @@
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1315,7 +1278,7 @@
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1330,7 +1293,7 @@
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1345,7 +1308,7 @@
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1360,7 +1323,7 @@
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1383,8 +1346,8 @@
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>33</v>
+      <c r="A31" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1399,7 +1362,7 @@
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -1414,7 +1377,7 @@
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -1438,7 +1401,7 @@
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1453,7 +1416,7 @@
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1547,31 +1510,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11D01E5-4373-4DAD-AA18-4DB1BB006D5A}">
-  <dimension ref="A1:G53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37E1B8-0EDD-4932-9EE1-20FA5689318C}">
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="37.375" style="2" customWidth="1"/>
-    <col min="4" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="15.625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1599,13 +1564,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="22">
-        <v>44436</v>
+        <v>44438</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1615,26 +1580,26 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1668,10 +1633,10 @@
     </row>
     <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -1681,10 +1646,10 @@
     </row>
     <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1694,10 +1659,10 @@
     </row>
     <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1707,10 +1672,10 @@
     </row>
     <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1720,10 +1685,10 @@
     </row>
     <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -1731,132 +1696,126 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="27">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="27">
-        <v>0</v>
-      </c>
-      <c r="E22" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="27">
-        <v>1</v>
-      </c>
-      <c r="E23" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="13"/>
+    <row r="22" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="24">
-        <v>44440</v>
+        <v>44436</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="13"/>
@@ -1871,23 +1830,23 @@
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>32</v>
+      <c r="A26" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E26" s="24">
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1895,49 +1854,43 @@
         <v>1</v>
       </c>
       <c r="E27" s="24">
-        <v>44437</v>
+        <v>44436</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="27">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E28" s="24">
-        <v>44437</v>
+        <v>44440</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="27">
-        <v>0</v>
-      </c>
-      <c r="E29" s="24">
-        <v>44438</v>
-      </c>
+      <c r="D29" s="27"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="24"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>36</v>
+      <c r="A30" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="27">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E30" s="24">
         <v>44439</v>
@@ -1946,32 +1899,38 @@
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="28">
-        <v>0</v>
-      </c>
-      <c r="E31" s="25">
-        <v>44439</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="A31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="27">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+      <c r="A32" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="24"/>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24">
+        <v>44437</v>
+      </c>
       <c r="F32" s="24"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -1979,40 +1938,40 @@
         <v>0</v>
       </c>
       <c r="E33" s="24">
-        <v>44440</v>
+        <v>44438</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
       <c r="D34" s="27">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E34" s="24">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="27">
-        <v>0</v>
-      </c>
-      <c r="E35" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="28">
+        <v>0</v>
+      </c>
+      <c r="E35" s="25">
+        <v>44439</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -2024,70 +1983,88 @@
       <c r="G36" s="13"/>
     </row>
     <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="27">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="27">
+        <v>0</v>
+      </c>
+      <c r="E38" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="27">
+        <v>0</v>
+      </c>
+      <c r="E39" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="28">
+        <v>0</v>
+      </c>
+      <c r="E41" s="25">
+        <v>44440</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="28">
-        <v>0</v>
-      </c>
-      <c r="E37" s="25">
-        <v>44440</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="28">
-        <v>0</v>
-      </c>
-      <c r="E38" s="25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="28">
+        <v>0</v>
+      </c>
+      <c r="E42" s="25">
         <v>44441</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-    </row>
-    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
@@ -2098,624 +2075,6 @@
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E5:G6"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"&amp;10Status Report&amp;R&amp;"Arial,Regular"&amp;8v1.0</oddHeader>
-    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;8&amp;G_x000D_Copyright 2018 GoLeanSixSigma.com. All Rights Reserved.</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2755D9C-88E6-44E4-9B88-8D336F63A0A1}">
-  <dimension ref="A1:G58"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.375" style="2" customWidth="1"/>
-    <col min="4" max="7" width="15.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="22">
-        <v>44436</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27">
-        <v>1</v>
-      </c>
-      <c r="E19" s="34">
-        <v>44436</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="27">
-        <v>1</v>
-      </c>
-      <c r="E20" s="34">
-        <v>44436</v>
-      </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-    </row>
-    <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="32">
-        <v>44436</v>
-      </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="30">
-        <v>0</v>
-      </c>
-      <c r="E22" s="32">
-        <v>44436</v>
-      </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="31"/>
-    </row>
-    <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="30">
-        <v>0</v>
-      </c>
-      <c r="E23" s="32">
-        <v>44436</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="31"/>
-    </row>
-    <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40">
-        <v>0</v>
-      </c>
-      <c r="E24" s="41">
-        <v>44436</v>
-      </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="39"/>
-    </row>
-    <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="30">
-        <v>0</v>
-      </c>
-      <c r="E25" s="32">
-        <v>44436</v>
-      </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="31"/>
-    </row>
-    <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="27">
-        <v>1</v>
-      </c>
-      <c r="E26" s="34">
-        <v>44436</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="34">
-        <v>44437</v>
-      </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="27">
-        <v>1</v>
-      </c>
-      <c r="E28" s="34">
-        <v>44437</v>
-      </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
-    </row>
-    <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="40">
-        <v>0</v>
-      </c>
-      <c r="E29" s="41">
-        <v>44438</v>
-      </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="27">
-        <v>0</v>
-      </c>
-      <c r="E30" s="24">
-        <v>44438</v>
-      </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="27">
-        <v>0</v>
-      </c>
-      <c r="E31" s="24">
-        <v>44439</v>
-      </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="27">
-        <v>0</v>
-      </c>
-      <c r="E32" s="24">
-        <v>44439</v>
-      </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="27">
-        <v>0</v>
-      </c>
-      <c r="E33" s="24">
-        <v>44439</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="27">
-        <v>0</v>
-      </c>
-      <c r="E34" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="13"/>
-    </row>
-    <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="27">
-        <v>0</v>
-      </c>
-      <c r="E35" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="28">
-        <v>0</v>
-      </c>
-      <c r="E36" s="25">
-        <v>44440</v>
-      </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="27">
-        <v>0</v>
-      </c>
-      <c r="E37" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="27">
-        <v>0</v>
-      </c>
-      <c r="E38" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="27">
-        <v>0</v>
-      </c>
-      <c r="E39" s="24">
-        <v>44441</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="13"/>
-    </row>
-    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="14"/>
-    </row>
     <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
@@ -2752,37 +2111,25 @@
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
     </row>
-    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-    </row>
-    <row r="49" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+    </row>
+    <row r="49" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:G43">
-    <sortCondition ref="E19:E43"/>
-  </sortState>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="E5:G6"/>

</xml_diff>

<commit_message>
History and QuizResult pages are working with loading dynamic data in from database.
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14409204-5E83-4EE0-8CE0-BDD2F1A80399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A6ACB5-4807-4A81-BE5F-A76494F3DE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>Project</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>All unit tests passed</t>
+  </si>
+  <si>
+    <t>Service layer finished</t>
   </si>
 </sst>
 </file>
@@ -2160,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B34F0E-8B16-47B5-9E9A-4063316F3415}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2314,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -2324,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2333,8 +2336,12 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -2350,178 +2357,172 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+    <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F21" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="27">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="27">
+        <v>1</v>
+      </c>
+      <c r="E22" s="24">
+        <v>44436</v>
+      </c>
       <c r="F22" s="24"/>
       <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>30</v>
-      </c>
+      <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="27">
-        <v>0.65</v>
-      </c>
-      <c r="E23" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>25</v>
+      <c r="A24" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="27">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="E24" s="24">
-        <v>44436</v>
+        <v>44440</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="24">
-        <v>44440</v>
+        <v>44436</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="24"/>
+      <c r="D26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="24">
+        <v>44440</v>
+      </c>
       <c r="F26" s="24"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>31</v>
-      </c>
+      <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="27">
-        <v>0.72</v>
-      </c>
-      <c r="E27" s="24">
-        <v>44439</v>
-      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>26</v>
+      <c r="A28" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="27">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E28" s="24">
-        <v>44437</v>
+        <v>44439</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -2536,7 +2537,7 @@
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -2544,122 +2545,122 @@
         <v>1</v>
       </c>
       <c r="E30" s="24">
-        <v>44438</v>
+        <v>44437</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="27">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="24">
-        <v>44439</v>
+        <v>44438</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="E32" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="28">
-        <v>0.4</v>
-      </c>
-      <c r="E32" s="25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="E33" s="25">
         <v>44439</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>32</v>
-      </c>
+      <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E34" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>29</v>
+      <c r="A35" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="27">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E35" s="24">
-        <v>44438</v>
+        <v>44440</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="24">
-        <v>44440</v>
+        <v>44438</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="13"/>
     </row>
     <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
+      <c r="A37" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="24"/>
+      <c r="D37" s="27">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24">
+        <v>44440</v>
+      </c>
       <c r="F37" s="24"/>
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="28">
-        <v>0</v>
-      </c>
-      <c r="E38" s="25">
-        <v>44440</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2667,19 +2668,25 @@
         <v>0</v>
       </c>
       <c r="E39" s="25">
-        <v>44441</v>
+        <v>44440</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="A40" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="28">
+        <v>0</v>
+      </c>
+      <c r="E40" s="25">
+        <v>44441</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
@@ -2717,16 +2724,24 @@
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
     </row>
-    <row r="45" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+    </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2735,6 +2750,7 @@
     <row r="52" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
words are loading into webpage. still can't hide stems from examples and definitions. still haven't implemented saving attempt to db or checking guesses.
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A6ACB5-4807-4A81-BE5F-A76494F3DE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F47E43-5FA7-49B8-934A-5DC77D123CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
   <si>
     <t>Project</t>
   </si>
@@ -248,6 +248,21 @@
   </si>
   <si>
     <t>Service layer finished</t>
+  </si>
+  <si>
+    <t>Possible that "vis" field (holds example sentences) from JSON response is not populated for several entries</t>
+  </si>
+  <si>
+    <t>Difficulties parsing JSON response to get a couple fields (but they are indeed in the response)</t>
+  </si>
+  <si>
+    <t>Work through parsing a String of JSON response without making new API calls</t>
+  </si>
+  <si>
+    <t>Investigate a larger set of data to see if this actually the case or just small sample size. May need to discuss removing example sentence feature</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -484,7 +499,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -584,6 +599,24 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -2163,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B34F0E-8B16-47B5-9E9A-4063316F3415}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2216,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="22">
-        <v>44440</v>
+        <v>44439</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
@@ -2393,82 +2426,86 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A19" s="39">
+        <v>1</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
+        <v>2</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="35"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="27">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="27">
-        <v>0.65</v>
-      </c>
-      <c r="E24" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -2482,238 +2519,250 @@
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E26" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D26" s="27"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="27">
+        <v>0.65</v>
+      </c>
+      <c r="E27" s="24">
+        <v>44440</v>
+      </c>
       <c r="F27" s="24"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>31</v>
+      <c r="A28" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="27">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E28" s="24">
-        <v>44439</v>
+        <v>44436</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="27">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="24">
-        <v>44437</v>
+        <v>44440</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="27">
-        <v>1</v>
-      </c>
-      <c r="E30" s="24">
-        <v>44437</v>
-      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>28</v>
+      <c r="A31" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="27">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E31" s="24">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="27">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="24">
-        <v>44439</v>
+        <v>44437</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="28">
-        <v>0.8</v>
-      </c>
-      <c r="E33" s="25">
-        <v>44439</v>
-      </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="A33" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="27">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F33" s="24"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="27">
+        <v>1</v>
+      </c>
+      <c r="E34" s="24">
+        <v>44438</v>
+      </c>
       <c r="F34" s="24"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>32</v>
+      <c r="A35" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="27">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E35" s="24">
-        <v>44440</v>
+        <v>44439</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="27">
-        <v>1</v>
-      </c>
-      <c r="E36" s="24">
-        <v>44438</v>
-      </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="13"/>
+      <c r="A36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="E36" s="25">
+        <v>44439</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="27">
-        <v>0</v>
-      </c>
-      <c r="E37" s="24">
-        <v>44440</v>
-      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="24"/>
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+      <c r="A38" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E38" s="24">
+        <v>44440</v>
+      </c>
       <c r="F38" s="24"/>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="27">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="E40" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="28">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="28">
         <v>0</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E42" s="25">
         <v>44440</v>
       </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="28">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="28">
         <v>0</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E43" s="25">
         <v>44441</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-    </row>
-    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
@@ -2733,28 +2782,63 @@
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
     </row>
-    <row r="46" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+    </row>
+    <row r="49" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="E5:G6"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="F21:G22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version 1 Complete. Fully functional, but still needs work on aesthetics and performance.
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F47E43-5FA7-49B8-934A-5DC77D123CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5A39C0-6650-43FF-B15B-DE9641905FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Report 8-27" sheetId="1" r:id="rId1"/>
     <sheet name="Status Report 8-30" sheetId="5" r:id="rId2"/>
     <sheet name="Status Report 8-31" sheetId="6" r:id="rId3"/>
+    <sheet name="Status Report 9-1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="62">
   <si>
     <t>Project</t>
   </si>
@@ -263,6 +264,27 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Refactored a lot of code to better follow MVC design</t>
+  </si>
+  <si>
+    <t>Revised Word model to better follow format of API call</t>
+  </si>
+  <si>
+    <t>Revised DAO and Service layer to accommodate above changes</t>
+  </si>
+  <si>
+    <t>Passed regression tests</t>
+  </si>
+  <si>
+    <t>Webpages are functional!</t>
+  </si>
+  <si>
+    <t>Resolved issues with JSON parsing</t>
   </si>
 </sst>
 </file>
@@ -499,7 +521,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -600,23 +622,26 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="16" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -2198,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B34F0E-8B16-47B5-9E9A-4063316F3415}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2426,56 +2451,56 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="37">
         <v>1</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38" t="s">
+      <c r="C19" s="36"/>
+      <c r="D19" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="39"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
+      <c r="A21" s="39">
         <v>2</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="35" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35" t="s">
+      <c r="E21" s="39"/>
+      <c r="F21" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="35"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -2849,4 +2874,667 @@
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF44962-D0FD-4C53-B9E9-97B6FBB8B6DE}">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22">
+        <v>44440</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+    </row>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37">
+        <v>1</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="37"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="39">
+        <v>2</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+    </row>
+    <row r="23" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="27">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24">
+        <v>44436</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="27">
+        <v>0.85</v>
+      </c>
+      <c r="E27" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+    </row>
+    <row r="28" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="27">
+        <v>1</v>
+      </c>
+      <c r="E28" s="24">
+        <v>44436</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="E29" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="27">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+    </row>
+    <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="27">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F33" s="24"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="27">
+        <v>1</v>
+      </c>
+      <c r="E34" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F34" s="24"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="27">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24">
+        <v>44439</v>
+      </c>
+      <c r="F35" s="24"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="28">
+        <v>1</v>
+      </c>
+      <c r="E36" s="25">
+        <v>44439</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="27">
+        <v>0.85</v>
+      </c>
+      <c r="E38" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="27">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="E40" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="28">
+        <v>0</v>
+      </c>
+      <c r="E42" s="25">
+        <v>44440</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="28">
+        <v>0</v>
+      </c>
+      <c r="E43" s="25">
+        <v>44441</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+    </row>
+    <row r="49" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E5:G6"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="F19:G20"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"&amp;10Status Report&amp;R&amp;"Arial,Regular"&amp;8v1.0</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;8&amp;G_x000D_Copyright 2018 GoLeanSixSigma.com. All Rights Reserved.</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Version - Revised hideWord method in serviceImpl
</commit_message>
<xml_diff>
--- a/mgmt-documents/AW_status.xlsx
+++ b/mgmt-documents/AW_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Austin\mthree\repos\final-project-repo-austinwongdev\mgmt-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52417C6-9D4D-4ECD-89E8-745441876500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340CB128-A8F8-4F9C-9F00-E97BE0FBA291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="73">
   <si>
     <t>Project</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>Tested program in Firefox and Chrome</t>
+  </si>
+  <si>
+    <t>Separated API key from application code</t>
+  </si>
+  <si>
+    <t>Displayed variants alongside word guesses in details view</t>
+  </si>
+  <si>
+    <t>Added delete confirmation dialog in history view</t>
+  </si>
+  <si>
+    <t>Made incorrectly spelled words easier to see in details view</t>
   </si>
 </sst>
 </file>
@@ -3537,18 +3549,18 @@
     <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E5:G6"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="F19:G20"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:C22"/>
     <mergeCell ref="D21:E22"/>
     <mergeCell ref="F21:G22"/>
     <mergeCell ref="F27:G27"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E5:G6"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="F19:G20"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>
@@ -3563,10 +3575,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46E0591-0B1D-41BC-8B4F-DBB7AE05AB38}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="113" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3616,7 +3628,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="22">
-        <v>44440</v>
+        <v>44441</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
@@ -3775,175 +3787,173 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12" t="s">
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37">
+    <row r="24" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37">
         <v>1</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B24" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36" t="s">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37" t="s">
+      <c r="E24" s="36"/>
+      <c r="F24" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="37"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="G24" s="37"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="39">
         <v>2</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B26" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="39" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39" t="s">
+      <c r="E26" s="39"/>
+      <c r="F26" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-    </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="G26" s="39"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E29" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F29" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="27">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="27">
-        <v>1</v>
-      </c>
-      <c r="E28" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-    </row>
-    <row r="29" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="27">
-        <v>1</v>
-      </c>
-      <c r="E29" s="24">
-        <v>44436</v>
-      </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3951,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="24">
-        <v>44440</v>
+        <v>44436</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="13"/>
@@ -3965,9 +3975,9 @@
       <c r="F31" s="24"/>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3975,14 +3985,14 @@
         <v>1</v>
       </c>
       <c r="E32" s="24">
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="F32" s="40"/>
       <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3990,14 +4000,14 @@
         <v>1</v>
       </c>
       <c r="E33" s="24">
-        <v>44437</v>
+        <v>44436</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -4005,29 +4015,23 @@
         <v>1</v>
       </c>
       <c r="E34" s="24">
-        <v>44437</v>
+        <v>44440</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="27">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24">
-        <v>44438</v>
-      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="24"/>
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>35</v>
+      <c r="A36" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -4037,36 +4041,42 @@
       <c r="E36" s="24">
         <v>44439</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="13"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
     </row>
     <row r="37" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="28">
+      <c r="A37" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="27">
         <v>1</v>
       </c>
-      <c r="E37" s="25">
-        <v>44439</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="E37" s="24">
+        <v>44437</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+      <c r="A38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="27">
+        <v>1</v>
+      </c>
+      <c r="E38" s="24">
+        <v>44437</v>
+      </c>
       <c r="F38" s="24"/>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
-        <v>32</v>
+      <c r="A39" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -4074,14 +4084,14 @@
         <v>1</v>
       </c>
       <c r="E39" s="24">
-        <v>44440</v>
+        <v>44438</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -4089,25 +4099,25 @@
         <v>1</v>
       </c>
       <c r="E40" s="24">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="27">
+      <c r="A41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="28">
         <v>1</v>
       </c>
-      <c r="E41" s="24">
-        <v>44440</v>
-      </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="13"/>
+      <c r="E41" s="25">
+        <v>44439</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -4119,70 +4129,88 @@
       <c r="G42" s="13"/>
     </row>
     <row r="43" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="27">
+        <v>1</v>
+      </c>
+      <c r="E43" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F43" s="24"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="27">
+        <v>1</v>
+      </c>
+      <c r="E44" s="24">
+        <v>44438</v>
+      </c>
+      <c r="F44" s="24"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="27">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24">
+        <v>44440</v>
+      </c>
+      <c r="F45" s="24"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="28">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="28">
         <v>1</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E47" s="25">
         <v>44440</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-    </row>
-    <row r="44" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="28">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="28">
         <v>0</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E48" s="25">
         <v>44441</v>
       </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-    </row>
-    <row r="47" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
     </row>
     <row r="49" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
@@ -4193,38 +4221,74 @@
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
     </row>
-    <row r="50" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+    </row>
+    <row r="51" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+    </row>
+    <row r="52" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+    </row>
+    <row r="53" spans="1:7" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+    </row>
+    <row r="54" spans="1:7" s="21" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+    </row>
     <row r="55" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="E5:G6"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:G23"/>
-    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:G27"/>
+    <mergeCell ref="F32:G32"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.3"/>

</xml_diff>